<commit_message>
separate data training and testing
</commit_message>
<xml_diff>
--- a/iris-data.xlsx
+++ b/iris-data.xlsx
@@ -123,15 +123,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:M156"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H95" activeCellId="0" sqref="H95"/>
+      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -153,6 +154,24 @@
       <c r="F1" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H1" s="0" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -173,6 +192,24 @@
       <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H2" s="0" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -193,6 +230,24 @@
       <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H3" s="0" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -213,6 +268,24 @@
       <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H4" s="0" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -233,6 +306,24 @@
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H5" s="0" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -253,6 +344,24 @@
       <c r="F6" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -273,6 +382,24 @@
       <c r="F7" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -293,6 +420,24 @@
       <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H8" s="0" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -313,6 +458,24 @@
       <c r="F9" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H9" s="0" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -333,6 +496,24 @@
       <c r="F10" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H10" s="0" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -353,6 +534,24 @@
       <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H11" s="0" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -1016,102 +1215,102 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>5.1</v>
+        <v>5.7</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>1.9</v>
+        <v>4.5</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>0.4</v>
+        <v>1.3</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>4.8</v>
+        <v>6.3</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>1.4</v>
+        <v>4.7</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>0.3</v>
+        <v>1.6</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>5.1</v>
+        <v>4.9</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>3.8</v>
+        <v>2.4</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>1.6</v>
+        <v>3.3</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="C48" s="0" t="n">
         <v>4.6</v>
       </c>
-      <c r="B48" s="0" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="C48" s="0" t="n">
-        <v>1.4</v>
-      </c>
       <c r="D48" s="0" t="n">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>3.7</v>
+        <v>2.7</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>1.5</v>
+        <v>3.9</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,33 +1318,33 @@
         <v>5</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>3.3</v>
+        <v>2</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>1.4</v>
+        <v>3.5</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>7</v>
+        <v>5.9</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>4.7</v>
+        <v>4.2</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>1</v>
@@ -1156,16 +1355,16 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>6.4</v>
+        <v>6</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>3.2</v>
+        <v>2.2</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>1</v>
@@ -1176,16 +1375,16 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>6.9</v>
+        <v>6.1</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>4.9</v>
+        <v>4.7</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>1</v>
@@ -1196,13 +1395,13 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>5.5</v>
+        <v>5.6</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>1.3</v>
@@ -1216,16 +1415,16 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>4.6</v>
+        <v>4.4</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>1</v>
@@ -1236,16 +1435,16 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>5.7</v>
+        <v>5.6</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>4.5</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>1</v>
@@ -1256,16 +1455,16 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>6.3</v>
+        <v>5.8</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>4.7</v>
+        <v>4.1</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>1</v>
@@ -1276,16 +1475,16 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>4.9</v>
+        <v>6.2</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>3.3</v>
+        <v>4.5</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E58" s="0" t="s">
         <v>1</v>
@@ -1296,16 +1495,16 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>6.6</v>
+        <v>5.6</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>4.6</v>
+        <v>3.9</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="E59" s="0" t="s">
         <v>1</v>
@@ -1316,16 +1515,16 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>5.2</v>
+        <v>5.9</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>3.9</v>
+        <v>4.8</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>1</v>
@@ -1336,16 +1535,16 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>5</v>
+        <v>6.1</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>1</v>
@@ -1356,13 +1555,13 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>5.9</v>
+        <v>6.3</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>4.2</v>
+        <v>4.9</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>1.5</v>
@@ -1376,16 +1575,16 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>6</v>
+        <v>6.1</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>4</v>
+        <v>4.7</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E63" s="0" t="s">
         <v>1</v>
@@ -1396,16 +1595,16 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>6.1</v>
+        <v>6.4</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>2.9</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E64" s="0" t="s">
         <v>1</v>
@@ -1416,16 +1615,16 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>5.6</v>
+        <v>6.6</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>3.6</v>
+        <v>4.4</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>1</v>
@@ -1436,13 +1635,13 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>4.4</v>
+        <v>4.8</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>1.4</v>
@@ -1456,16 +1655,16 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>5.6</v>
+        <v>6.7</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="E67" s="0" t="s">
         <v>1</v>
@@ -1476,16 +1675,16 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>4.1</v>
+        <v>4.5</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>1</v>
@@ -1496,16 +1695,16 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>6.2</v>
+        <v>5.7</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>2.2</v>
+        <v>2.6</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E69" s="0" t="s">
         <v>1</v>
@@ -1516,13 +1715,13 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>1.1</v>
@@ -1536,16 +1735,16 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>3.2</v>
+        <v>2.4</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>4.8</v>
+        <v>3.7</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="E71" s="0" t="s">
         <v>1</v>
@@ -1556,16 +1755,16 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E72" s="0" t="s">
         <v>1</v>
@@ -1576,16 +1775,16 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>6.3</v>
+        <v>6</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>4.9</v>
+        <v>5.1</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>1</v>
@@ -1596,16 +1795,16 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>6.1</v>
+        <v>5.4</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>1</v>
@@ -1616,16 +1815,16 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>6.4</v>
+        <v>6</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
       <c r="E75" s="0" t="s">
         <v>1</v>
@@ -1636,16 +1835,16 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>4.4</v>
+        <v>4.7</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>1</v>
@@ -1656,16 +1855,16 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>2.8</v>
+        <v>2.3</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>4.8</v>
+        <v>4.4</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E77" s="0" t="s">
         <v>1</v>
@@ -1676,16 +1875,16 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>6.7</v>
+        <v>5.6</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>5</v>
+        <v>4.1</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E78" s="0" t="s">
         <v>1</v>
@@ -1696,16 +1895,16 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E79" s="0" t="s">
         <v>1</v>
@@ -1716,16 +1915,16 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>2.6</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>3.5</v>
+        <v>4.4</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E80" s="0" t="s">
         <v>1</v>
@@ -1736,16 +1935,16 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>3.8</v>
+        <v>4.6</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>1.1</v>
+        <v>1.4</v>
       </c>
       <c r="E81" s="0" t="s">
         <v>1</v>
@@ -1756,16 +1955,16 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>5.5</v>
+        <v>5.8</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>3.7</v>
+        <v>4</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E82" s="0" t="s">
         <v>1</v>
@@ -1776,16 +1975,16 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>5.8</v>
+        <v>5</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>2.7</v>
+        <v>2.3</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>3.9</v>
+        <v>3.3</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>1</v>
@@ -1796,16 +1995,16 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>2.7</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>5.1</v>
+        <v>4.2</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>1</v>
@@ -1816,16 +2015,16 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>5.4</v>
+        <v>5.7</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>1</v>
@@ -1836,16 +2035,16 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>6</v>
+        <v>5.7</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>3.4</v>
+        <v>2.9</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="E86" s="0" t="s">
         <v>1</v>
@@ -1856,16 +2055,16 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>4.7</v>
+        <v>4.3</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E87" s="0" t="s">
         <v>1</v>
@@ -1876,16 +2075,16 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
-        <v>6.3</v>
+        <v>5.1</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>4.4</v>
+        <v>3</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>1</v>
@@ -1896,10 +2095,10 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>4.1</v>
@@ -1914,226 +2113,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="B90" s="0" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="C90" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D90" s="0" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E90" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F90" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="B91" s="0" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="C91" s="0" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D91" s="0" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E91" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F91" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="B92" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C92" s="0" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D92" s="0" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F92" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="B93" s="0" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="C93" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D93" s="0" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E93" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F93" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B94" s="0" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="C94" s="0" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="D94" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E94" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F94" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="B95" s="0" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="C95" s="0" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="D95" s="0" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E95" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F95" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="B96" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C96" s="0" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="D96" s="0" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E96" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F96" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="B97" s="0" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="C97" s="0" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="D97" s="0" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E97" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F97" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B98" s="0" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="C98" s="0" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="D98" s="0" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E98" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F98" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="B99" s="0" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="C99" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D99" s="0" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E99" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F99" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="B100" s="0" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="C100" s="0" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="D100" s="0" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E100" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F100" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>